<commit_message>
convert joyce agents contacts
</commit_message>
<xml_diff>
--- a/AGENTS ANNA crm.xlsx
+++ b/AGENTS ANNA crm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\sudara\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\sudara\import-not-singed-contact-new-pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -11938,7 +11938,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11950,6 +11950,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -11984,16 +11992,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12297,7 +12308,7 @@
   <dimension ref="A1:I1111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12308,7 +12319,8 @@
     <col min="4" max="4" width="23.77734375" customWidth="1"/>
     <col min="5" max="5" width="45.21875" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="8" width="28.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="8" max="8" width="41.109375" customWidth="1"/>
     <col min="9" max="9" width="45.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12491,7 +12503,7 @@
       <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G12" t="s">
@@ -12796,7 +12808,7 @@
       <c r="E31" t="s">
         <v>124</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
         <v>125</v>
       </c>
       <c r="G31" t="s">
@@ -29829,7 +29841,7 @@
       <c r="D1098" t="s">
         <v>1401</v>
       </c>
-      <c r="F1098" t="s">
+      <c r="F1098" s="2" t="s">
         <v>3924</v>
       </c>
       <c r="G1098" t="s">
@@ -30055,6 +30067,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F12" r:id="rId1"/>
+    <hyperlink ref="F31" r:id="rId2"/>
+    <hyperlink ref="F1098" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>